<commit_message>
[Add] D40070/ W40070 [Modify] 50070 template/ W42011 by Lukas
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/50070.xlsx
+++ b/PhoenixCI/Excel_Template/50070.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Source\Repos\buckblader\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\RekindlePhoenixCI\PhoenixCI\bin\Debug\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6C5AC34-5DC8-4E42-99F3-03F5F0559E6B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14856DA3-87F7-47D9-BD70-3113658E0620}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="360" yWindow="285" windowWidth="20100" windowHeight="7455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="50070" sheetId="1" r:id="rId1"/>
+    <sheet name="每月獎勵活動成績得獎名單" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -264,7 +264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="180" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -297,6 +297,12 @@
       <color indexed="8"/>
       <name val="標楷體"/>
       <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
     </font>
     <font>
@@ -339,16 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -357,10 +354,19 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -703,7 +709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -764,4 +770,17 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>